<commit_message>
nor reads timeline data
</commit_message>
<xml_diff>
--- a/Excel/timeline.xlsx
+++ b/Excel/timeline.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="17">
   <si>
     <t>harmony</t>
   </si>
@@ -36,66 +36,48 @@
     <t>flute</t>
   </si>
   <si>
-    <t>wave</t>
+    <t>measure</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>4/4</t>
+    <phoneticPr fontId="1"/>
   </si>
   <si>
     <t>oboe</t>
-  </si>
-  <si>
-    <t>random</t>
-  </si>
-  <si>
-    <t>clarinet</t>
-  </si>
-  <si>
-    <t>rest</t>
-  </si>
-  <si>
-    <t>timpani</t>
-  </si>
-  <si>
-    <t>3/4</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>14/16</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>5/8</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>2/4</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>3/8</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>3/16</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>measure</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>wave(100, c3 c6)</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>horn</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>violin</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>viola</t>
-    <phoneticPr fontId="1"/>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>8/4</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>7/4</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>6/4</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>5/4</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>renda-d6-3</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>renda-d6-4</t>
+  </si>
+  <si>
+    <t>renda-d6-5</t>
+  </si>
+  <si>
+    <t>renda-d6-6</t>
+  </si>
+  <si>
+    <t>renda-d6-7</t>
   </si>
 </sst>
 </file>
@@ -154,8 +136,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
@@ -163,10 +149,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="7">
     <cellStyle name="ハイパーリンク" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="標準" xfId="0" builtinId="0"/>
     <cellStyle name="表示済みのハイパーリンク" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="6" builtinId="9" hidden="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
@@ -495,38 +485,35 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="12" defaultRowHeight="18" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1">
+    <row r="1" spans="1:6" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>14</v>
-      </c>
       <c r="F1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:6">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -545,115 +532,45 @@
       <c r="F2" t="s">
         <v>2</v>
       </c>
-      <c r="G2" t="s">
-        <v>3</v>
-      </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:6">
       <c r="A3" t="s">
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="C3" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="D3" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="E3" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="F3" t="s">
-        <v>5</v>
-      </c>
-      <c r="G3" t="s">
-        <v>5</v>
+        <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="C4" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="D4" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="E4" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="F4" t="s">
-        <v>5</v>
-      </c>
-      <c r="G4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7">
-      <c r="A5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E5" t="s">
-        <v>5</v>
-      </c>
-      <c r="F5" t="s">
-        <v>9</v>
-      </c>
-      <c r="G5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7">
-      <c r="A6" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6" t="s">
-        <v>7</v>
-      </c>
-      <c r="D6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E6" t="s">
-        <v>9</v>
-      </c>
-      <c r="F6" t="s">
-        <v>9</v>
-      </c>
-      <c r="G6" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7">
-      <c r="A7" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7">
-      <c r="A8" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7">
-      <c r="A9" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>